<commit_message>
Repository created for pizza delievery system project
</commit_message>
<xml_diff>
--- a/src/main/resources/rest-services.xlsx
+++ b/src/main/resources/rest-services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIYAMVAD\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED37DCA-23EB-4E15-B485-50659593AAD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707D58AB-4622-4454-BAA5-63A9A950AA24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{420ED039-64A4-44EE-925E-22693EDBA285}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t xml:space="preserve"> FOOD rest services   </t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>remove saved card details</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Method</t>
   </si>
 </sst>
 </file>
@@ -592,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5257770C-153E-4746-BFF5-05EBB845E977}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,15 +616,16 @@
     <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
     <col min="4" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -628,16 +641,28 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -651,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -665,7 +690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -679,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -687,7 +712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -698,7 +723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -709,7 +734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -717,7 +742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -725,12 +750,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -741,7 +766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -752,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Repository Created For Pizza-delievery-system project
</commit_message>
<xml_diff>
--- a/src/main/resources/rest-services.xlsx
+++ b/src/main/resources/rest-services.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIYAMVAD\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder (8)\Pizza-Delievery-System\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707D58AB-4622-4454-BAA5-63A9A950AA24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88740D90-222E-4BDB-8D05-605C130EE1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{420ED039-64A4-44EE-925E-22693EDBA285}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
   <si>
     <t xml:space="preserve"> FOOD rest services   </t>
   </si>
@@ -250,6 +250,30 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deeptansu </t>
+  </si>
+  <si>
+    <t>Anuj</t>
+  </si>
+  <si>
+    <t>Subham</t>
+  </si>
+  <si>
+    <t>Pratyush</t>
+  </si>
+  <si>
+    <t>Satwik</t>
+  </si>
+  <si>
+    <t>Suraj</t>
+  </si>
+  <si>
+    <t>Priyamvad</t>
+  </si>
+  <si>
+    <t>Team members</t>
   </si>
 </sst>
 </file>
@@ -604,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5257770C-153E-4746-BFF5-05EBB845E977}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,15 +641,16 @@
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
     <col min="4" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -650,8 +675,11 @@
       <c r="H2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -661,8 +689,11 @@
       <c r="F4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -675,8 +706,11 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -689,8 +723,11 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -703,16 +740,22 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -722,8 +765,11 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -733,8 +779,11 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -742,7 +791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -750,12 +799,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -765,8 +814,11 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -776,8 +828,11 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -790,8 +845,11 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -804,8 +862,11 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -818,13 +879,16 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -837,8 +901,11 @@
       <c r="E22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -848,24 +915,33 @@
       <c r="D23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
       <c r="E25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -878,8 +954,11 @@
       <c r="E26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -892,8 +971,11 @@
       <c r="E27" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -906,8 +988,11 @@
       <c r="E28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -920,8 +1005,11 @@
       <c r="E29" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -934,8 +1022,11 @@
       <c r="E30" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -945,8 +1036,11 @@
       <c r="E31" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -956,8 +1050,11 @@
       <c r="E32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -967,8 +1064,11 @@
       <c r="E33" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -981,8 +1081,11 @@
       <c r="E34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -995,8 +1098,11 @@
       <c r="E35" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1009,13 +1115,16 @@
       <c r="E36" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -1023,7 +1132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -1031,7 +1140,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1039,7 +1148,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>

</xml_diff>